<commit_message>
Added first draft of examples in Excel
</commit_message>
<xml_diff>
--- a/Output/Table2.xlsx
+++ b/Output/Table2.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -578,21 +578,49 @@
         <v>43916</v>
       </c>
       <c r="C8">
+        <v>0.09217945242613174</v>
+      </c>
+      <c r="D8">
+        <v>0.04955177567938374</v>
+      </c>
+      <c r="E8">
+        <v>-0.004335454964670524</v>
+      </c>
+      <c r="F8">
+        <v>0.05388723064405426</v>
+      </c>
+      <c r="G8">
+        <v>0.07446332850061535</v>
+      </c>
+      <c r="H8">
+        <v>0.9255366714993846</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="B9" s="2">
+        <v>43916</v>
+      </c>
+      <c r="C9">
         <v>0.09630539297713012</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>0.05367771623038212</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>-0.001568691807165634</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>0.05524640803754775</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>0.02761047347365702</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>0.9723895265263429</v>
       </c>
     </row>

</xml_diff>